<commit_message>
LITE-28847: Support 'late' field in product capabilities
</commit_message>
<xml_diff>
--- a/tests/fixtures/capabilities_sync.xlsx
+++ b/tests/fixtures/capabilities_sync.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc1/Documents/Connect/connect-cli/tests/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rselekh00/Development/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7BF8E9-47B9-5A47-9059-036B4C40920E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869DF530-BE9C-CE4A-B970-5E35F24DCEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Product information</t>
   </si>
@@ -150,12 +150,15 @@
   <si>
     <t>Administrative Hold</t>
   </si>
+  <si>
+    <t>Pay-as-you-go late charges support</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,19 +170,23 @@
       <sz val="24"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -539,19 +546,19 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
     <col min="2" max="2" width="180" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="31">
+    <row r="1" spans="1:2" ht="31" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="3" spans="1:2" ht="16">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -559,7 +566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -567,7 +574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -575,7 +582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -583,7 +590,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16">
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -591,7 +598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -599,7 +606,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="19">
+    <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -607,7 +614,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="34">
+    <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -615,7 +622,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="404">
+    <row r="11" spans="1:2" ht="404" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
@@ -623,7 +630,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17">
+    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -631,7 +638,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="32">
+    <row r="13" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -654,19 +661,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>23</v>
       </c>
@@ -677,7 +684,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -688,7 +695,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -699,7 +706,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -710,84 +717,95 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B11" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"-,create,update,delete"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Disabled,QT,TR,PR"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3 C4 C5 C6 C7 C9 C10" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C10:C11 C3:C8" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Disabled,Enabled"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Disabled,1,2"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>